<commit_message>
run simulation in one file
</commit_message>
<xml_diff>
--- a/DataProcessed/samplesize200partition.xlsx
+++ b/DataProcessed/samplesize200partition.xlsx
@@ -32,16 +32,16 @@
     <t xml:space="preserve">0.3</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0898 (0.0032)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8278 (0.0476)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8302 (0.0882)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8224 (0.1001)</t>
+    <t xml:space="preserve">0.0899 (0.0033)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8273 (0.0481)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8295 (0.0897)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8222 (0.1015)</t>
   </si>
   <si>
     <t xml:space="preserve">0.5</t>
@@ -50,13 +50,13 @@
     <t xml:space="preserve">0.0900 (0.0028)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.8288 (0.0471)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8296 (0.0812)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8271 (0.1006)</t>
+    <t xml:space="preserve">0.8290 (0.0468)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8299 (0.0808)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8271 (0.1012)</t>
   </si>
   <si>
     <t xml:space="preserve">0.8</t>
@@ -65,13 +65,13 @@
     <t xml:space="preserve">0.0899 (0.0024)</t>
   </si>
   <si>
-    <t xml:space="preserve">0.8319 (0.0629)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8341 (0.0901)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8268 (0.1247)</t>
+    <t xml:space="preserve">0.8319 (0.0626)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8340 (0.0897)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8272 (0.1243)</t>
   </si>
 </sst>
 </file>

</xml_diff>